<commit_message>
added file via upload
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/EmployeeListData.xlsx
+++ b/src/main/resources/testdata/EmployeeListData.xlsx
@@ -3,15 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{71B62372-02A1-46BD-93A0-CE394CB3767C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B1D452-6803-431E-9DBA-422644E65F35}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17304" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>0001</t>
   </si>
@@ -168,6 +167,24 @@
   </si>
   <si>
     <t>0006</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>Paresh</t>
+  </si>
+  <si>
+    <t>Sonaawane</t>
+  </si>
+  <si>
+    <t>Test Analyst</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Sunil Dolwani</t>
   </si>
 </sst>
 </file>
@@ -486,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF9FC9C-61C0-4B3D-BC71-98BEC58AAD54}">
-  <dimension ref="B1:H9"/>
+  <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,6 +719,29 @@
         <v>6</v>
       </c>
     </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>